<commit_message>
Project LMB_GHI is saved. Null issues is fixed. Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/LMB_GHI/LMB GHI Rating Model.xlsx
+++ b/DESIGN/rules/LMB_GHI/LMB GHI Rating Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="-285" windowWidth="14910" windowHeight="13740" tabRatio="726" activeTab="2"/>
+    <workbookView xWindow="14520" yWindow="-285" windowWidth="14910" windowHeight="11760" tabRatio="726" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Domain Model" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="300">
   <si>
     <t>Air Ambulance</t>
   </si>
@@ -1574,6 +1574,15 @@
   </si>
   <si>
     <t>Hospital Conf - Non-Metro Area</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>org.openl.rules.binding.MulDivNullToOneOperators.*</t>
+  </si>
+  <si>
+    <t>//Environment</t>
   </si>
 </sst>
 </file>
@@ -2161,6 +2170,9 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2172,9 +2184,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2485,8 +2494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K82"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -2516,11 +2525,11 @@
     </row>
     <row r="4" spans="3:8">
       <c r="C4" s="10"/>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="3:8">
@@ -2756,11 +2765,11 @@
     </row>
     <row r="24" spans="3:11">
       <c r="C24" s="10"/>
-      <c r="D24" s="81" t="s">
+      <c r="D24" s="82" t="s">
         <v>168</v>
       </c>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
       <c r="G24" s="10"/>
       <c r="H24" s="48"/>
       <c r="I24" s="48"/>
@@ -2937,11 +2946,11 @@
     </row>
     <row r="37" spans="3:11">
       <c r="C37" s="10"/>
-      <c r="D37" s="81" t="s">
+      <c r="D37" s="82" t="s">
         <v>169</v>
       </c>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
       <c r="G37" s="10"/>
       <c r="H37" s="48"/>
       <c r="I37" s="48"/>
@@ -3077,11 +3086,11 @@
     </row>
     <row r="48" spans="3:11">
       <c r="C48" s="10"/>
-      <c r="D48" s="81" t="s">
+      <c r="D48" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="E48" s="81"/>
-      <c r="F48" s="81"/>
+      <c r="E48" s="82"/>
+      <c r="F48" s="82"/>
       <c r="G48" s="10"/>
       <c r="H48" s="72"/>
     </row>
@@ -3130,11 +3139,11 @@
     </row>
     <row r="54" spans="2:8">
       <c r="C54" s="10"/>
-      <c r="D54" s="81" t="s">
+      <c r="D54" s="82" t="s">
         <v>219</v>
       </c>
-      <c r="E54" s="81"/>
-      <c r="F54" s="81"/>
+      <c r="E54" s="82"/>
+      <c r="F54" s="82"/>
       <c r="G54" s="10"/>
       <c r="H54" s="72"/>
     </row>
@@ -3195,11 +3204,11 @@
     <row r="61" spans="2:8" ht="15">
       <c r="B61"/>
       <c r="C61" s="10"/>
-      <c r="D61" s="81" t="s">
+      <c r="D61" s="82" t="s">
         <v>268</v>
       </c>
-      <c r="E61" s="81"/>
-      <c r="F61" s="81"/>
+      <c r="E61" s="82"/>
+      <c r="F61" s="82"/>
       <c r="G61" s="10"/>
       <c r="H61"/>
     </row>
@@ -3272,11 +3281,11 @@
     <row r="68" spans="2:8" ht="15">
       <c r="B68"/>
       <c r="C68" s="10"/>
-      <c r="D68" s="81" t="s">
+      <c r="D68" s="82" t="s">
         <v>274</v>
       </c>
-      <c r="E68" s="81"/>
-      <c r="F68" s="81"/>
+      <c r="E68" s="82"/>
+      <c r="F68" s="82"/>
       <c r="G68" s="10"/>
       <c r="H68"/>
     </row>
@@ -3361,11 +3370,11 @@
     </row>
     <row r="76" spans="2:8">
       <c r="C76" s="10"/>
-      <c r="D76" s="81" t="s">
+      <c r="D76" s="82" t="s">
         <v>289</v>
       </c>
-      <c r="E76" s="81"/>
-      <c r="F76" s="81"/>
+      <c r="E76" s="82"/>
+      <c r="F76" s="82"/>
       <c r="G76" s="10"/>
     </row>
     <row r="77" spans="2:8">
@@ -3637,7 +3646,7 @@
     </row>
     <row r="28" spans="3:5" ht="14.25" thickBot="1">
       <c r="C28" s="10"/>
-      <c r="D28" s="85" t="s">
+      <c r="D28" s="81" t="s">
         <v>265</v>
       </c>
       <c r="E28" s="10"/>
@@ -4974,7 +4983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
@@ -5351,10 +5360,10 @@
     </row>
     <row r="50" spans="3:6">
       <c r="C50" s="34"/>
-      <c r="D50" s="82" t="s">
+      <c r="D50" s="83" t="s">
         <v>212</v>
       </c>
-      <c r="E50" s="82"/>
+      <c r="E50" s="83"/>
       <c r="F50" s="35"/>
     </row>
     <row r="51" spans="3:6">
@@ -5417,10 +5426,10 @@
     </row>
     <row r="58" spans="3:6">
       <c r="C58" s="34"/>
-      <c r="D58" s="82" t="s">
+      <c r="D58" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="E58" s="82"/>
+      <c r="E58" s="83"/>
       <c r="F58" s="35"/>
     </row>
     <row r="59" spans="3:6">
@@ -5499,10 +5508,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F12"/>
+  <dimension ref="B1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -5540,10 +5549,10 @@
     <row r="5" spans="2:6">
       <c r="B5" s="66"/>
       <c r="C5" s="21"/>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="84" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="84"/>
+      <c r="E5" s="85"/>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6">
@@ -5594,6 +5603,19 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="66"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="D13" s="22" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="D14" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>298</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>